<commit_message>
working r2 but very slow
</commit_message>
<xml_diff>
--- a/lab3/Workbook1.xlsx
+++ b/lab3/Workbook1.xlsx
@@ -16,6 +16,26 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
+  <si>
+    <t>set size</t>
+  </si>
+  <si>
+    <t>r0 calls</t>
+  </si>
+  <si>
+    <t>log time</t>
+  </si>
+  <si>
+    <t>r1 calls</t>
+  </si>
+  <si>
+    <t>r2 calls</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -382,10 +402,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -393,84 +413,351 @@
     <col min="3" max="3" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1">
+    <row r="1" spans="1:13">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>8</v>
+      </c>
+      <c r="C2">
+        <f>LOG(B2)</f>
+        <v>0.90308998699194354</v>
+      </c>
+      <c r="D2">
+        <f>A2/C2</f>
+        <v>4.4292374598498165</v>
+      </c>
+      <c r="E2">
+        <v>6</v>
+      </c>
+      <c r="F2">
+        <f>LOG(E2)</f>
+        <v>0.77815125038364363</v>
+      </c>
+      <c r="G2">
+        <f>A2/F2</f>
+        <v>5.1403888357538747</v>
+      </c>
+      <c r="H2">
+        <v>3</v>
+      </c>
+      <c r="I2">
+        <f>LOG(H2)</f>
+        <v>0.47712125471966244</v>
+      </c>
+      <c r="J2">
+        <f>A2/I2</f>
+        <v>8.3836130971575393</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3">
+        <v>30</v>
+      </c>
+      <c r="B3">
         <v>19238</v>
       </c>
-      <c r="B1">
-        <v>30</v>
-      </c>
-      <c r="C1">
-        <f>1.618^B1</f>
-        <v>1859325.8971073017</v>
-      </c>
-      <c r="D1">
-        <f>LOG(A1,((1+SQRT(5))/2))</f>
-        <v>20.49958512031726</v>
-      </c>
-      <c r="E1">
-        <f>B1/D1</f>
-        <v>1.46344425137984</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2">
+      <c r="C3">
+        <f t="shared" ref="C3:C6" si="0">LOG(B3)</f>
+        <v>4.2841599203986815</v>
+      </c>
+      <c r="D3">
+        <f>A3/C3</f>
+        <v>7.0025397178003139</v>
+      </c>
+      <c r="E3">
+        <v>121</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F10" si="1">LOG(E3)</f>
+        <v>2.0827853703164503</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G10" si="2">A3/F3</f>
+        <v>14.403788516836912</v>
+      </c>
+      <c r="H3">
+        <v>33</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I10" si="3">LOG(H3)</f>
+        <v>1.5185139398778875</v>
+      </c>
+      <c r="J3">
+        <f t="shared" ref="J3:J8" si="4">A3/I3</f>
+        <v>19.756157129787347</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4">
+        <v>40</v>
+      </c>
+      <c r="B4">
         <v>157163</v>
-      </c>
-      <c r="B2">
-        <v>40</v>
-      </c>
-      <c r="C2">
-        <f t="shared" ref="C2:C4" si="0">1.618^B2</f>
-        <v>228633935.01716504</v>
-      </c>
-      <c r="D2">
-        <f>LOG(A2,((1+SQRT(5))/2))</f>
-        <v>24.864390564040846</v>
-      </c>
-      <c r="E2">
-        <f t="shared" ref="E2:E4" si="1">B2/D2</f>
-        <v>1.6087263388570012</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3">
-        <v>1057203</v>
-      </c>
-      <c r="B3">
-        <v>50</v>
-      </c>
-      <c r="C3">
-        <f t="shared" si="0"/>
-        <v>28114208661.730125</v>
-      </c>
-      <c r="D3">
-        <f>LOG(A3,((1+SQRT(5))/2))</f>
-        <v>28.825429004523318</v>
-      </c>
-      <c r="E3">
-        <f t="shared" si="1"/>
-        <v>1.7345795614057971</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4">
-        <v>8808978</v>
-      </c>
-      <c r="B4">
-        <v>60</v>
       </c>
       <c r="C4">
         <f t="shared" si="0"/>
-        <v>3457092791653.8726</v>
+        <v>5.1963503102327353</v>
       </c>
       <c r="D4">
-        <f>LOG(A4,((1+SQRT(5))/2))</f>
-        <v>33.23127395022415</v>
+        <f>A4/C4</f>
+        <v>7.6977104336540529</v>
       </c>
       <c r="E4">
+        <v>1438</v>
+      </c>
+      <c r="F4">
         <f t="shared" si="1"/>
-        <v>1.8055281326220505</v>
+        <v>3.1577588860468637</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="2"/>
+        <v>12.667211602743746</v>
+      </c>
+      <c r="H4">
+        <v>219</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="3"/>
+        <v>2.3404441148401185</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="4"/>
+        <v>17.09077339055904</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5">
+        <v>50</v>
+      </c>
+      <c r="B5">
+        <v>1057203</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>6.0241583868486224</v>
+      </c>
+      <c r="D5">
+        <f>A5/C5</f>
+        <v>8.2999145754791765</v>
+      </c>
+      <c r="E5">
+        <v>5690</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>3.7551122663950713</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="2"/>
+        <v>13.315181132520514</v>
+      </c>
+      <c r="H5">
+        <v>1051</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="3"/>
+        <v>3.0216027160282422</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="4"/>
+        <v>16.547509616261763</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6">
+        <v>60</v>
+      </c>
+      <c r="B6">
+        <v>8808978</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>6.9449255253579336</v>
+      </c>
+      <c r="D6">
+        <f>A6/C6</f>
+        <v>8.6394014998321627</v>
+      </c>
+      <c r="E6">
+        <v>32977</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>4.5182111442524908</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="2"/>
+        <v>13.279591874834043</v>
+      </c>
+      <c r="H6">
+        <v>5686</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="3"/>
+        <v>3.7548068553544232</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="4"/>
+        <v>15.979517006164752</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7">
+        <v>70</v>
+      </c>
+      <c r="E7">
+        <v>137559</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>5.1384890100108329</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="2"/>
+        <v>13.622681660625451</v>
+      </c>
+      <c r="H7">
+        <v>21991</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="3"/>
+        <v>4.3422449785471198</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="4"/>
+        <v>16.120693407634832</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8">
+        <v>80</v>
+      </c>
+      <c r="E8">
+        <v>576803</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>5.7610275105186846</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="2"/>
+        <v>13.886411730187577</v>
+      </c>
+      <c r="H8">
+        <v>87142</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="3"/>
+        <v>4.9402275232264987</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="4"/>
+        <v>16.193586150411026</v>
+      </c>
+      <c r="K8">
+        <v>3200</v>
+      </c>
+      <c r="L8">
+        <f>LOG(K8)</f>
+        <v>3.5051499783199058</v>
+      </c>
+      <c r="M8">
+        <f>A8/L8</f>
+        <v>22.823559760585688</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9">
+        <v>90</v>
+      </c>
+      <c r="E9">
+        <v>1935859</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>6.2868737219021442</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="2"/>
+        <v>14.315541234184321</v>
+      </c>
+      <c r="H9">
+        <v>261447</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="3"/>
+        <v>5.4173836628383816</v>
+      </c>
+      <c r="J9">
+        <f t="shared" ref="J9" si="5">A9/I9</f>
+        <v>16.613185552533942</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10">
+        <v>100</v>
+      </c>
+      <c r="E10">
+        <v>8038377</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>6.9051683707512845</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="2"/>
+        <v>14.481906107253973</v>
+      </c>
+      <c r="H10">
+        <v>1011144</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="3"/>
+        <v>6.0048130091538532</v>
+      </c>
+      <c r="J10">
+        <f t="shared" ref="J10" si="6">A10/I10</f>
+        <v>16.653307912762322</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13">
+        <v>130</v>
       </c>
     </row>
   </sheetData>

</xml_diff>